<commit_message>
Fixed issues with individual counties
</commit_message>
<xml_diff>
--- a/Data/IndividualCounties/12086.xlsx
+++ b/Data/IndividualCounties/12086.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">month</t>
   </si>
@@ -33,6 +33,33 @@
   </si>
   <si>
     <t xml:space="preserve">precip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grade_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grade_distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grade_visitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grade_encounters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEVER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RARELY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOMETIMES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FREQUENTLY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALWAYS</t>
   </si>
 </sst>
 </file>
@@ -386,13 +413,40 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2020</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2020</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -409,13 +463,40 @@
       <c r="G2" t="n">
         <v>0.000195079849505</v>
       </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1.023</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1.756</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2020</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>2020</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -432,13 +513,40 @@
       <c r="G3" t="n">
         <v>0.000290939571414</v>
       </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1.023</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1.756</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2020</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>2020</v>
       </c>
       <c r="C4" t="n">
         <v>68.4838709677419</v>
@@ -455,13 +563,40 @@
       <c r="G4" t="n">
         <v>0.000265658045862</v>
       </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1.023</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1.756</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2020</v>
+        <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>2020</v>
       </c>
       <c r="C5" t="n">
         <v>331.333333333333</v>
@@ -478,13 +613,40 @@
       <c r="G5" t="n">
         <v>0.000876543621132</v>
       </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1.023</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1.756</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2020</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>2020</v>
       </c>
       <c r="C6" t="n">
         <v>191.516129032258</v>
@@ -501,13 +663,40 @@
       <c r="G6" t="n">
         <v>0.00149387656785</v>
       </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1.023</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1.756</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2020</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>2020</v>
       </c>
       <c r="C7" t="n">
         <v>627.333333333333</v>
@@ -524,13 +713,40 @@
       <c r="G7" t="n">
         <v>0.0037315729756</v>
       </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1.023</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1.756</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2020</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>7</v>
+        <v>2020</v>
       </c>
       <c r="C8" t="n">
         <v>2633.61290322581</v>
@@ -547,13 +763,40 @@
       <c r="G8" t="n">
         <v>0.00647946028931</v>
       </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1.023</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1.756</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2020</v>
+        <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>2020</v>
       </c>
       <c r="C9" t="n">
         <v>1240.25806451613</v>
@@ -570,13 +813,40 @@
       <c r="G9" t="n">
         <v>0.00224880773203</v>
       </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1.023</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1.756</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2020</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>2020</v>
       </c>
       <c r="C10" t="n">
         <v>449.666666666667</v>
@@ -593,13 +863,40 @@
       <c r="G10" t="n">
         <v>0.00272050107509</v>
       </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1.023</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1.756</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2020</v>
+        <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>2020</v>
       </c>
       <c r="C11" t="n">
         <v>499.709677419355</v>
@@ -616,13 +913,40 @@
       <c r="G11" t="n">
         <v>0.00100497435778</v>
       </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1.023</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1.756</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2020</v>
+        <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>11</v>
+        <v>2020</v>
       </c>
       <c r="C12" t="n">
         <v>1457.56666666667</v>
@@ -639,13 +963,40 @@
       <c r="G12" t="n">
         <v>0.000335511912795</v>
       </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1.023</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="P12" t="n">
+        <v>1.756</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2020</v>
+        <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>12</v>
+        <v>2020</v>
       </c>
       <c r="C13" t="n">
         <v>2234.03225806452</v>
@@ -661,6 +1012,33 @@
       </c>
       <c r="G13" t="n">
         <v>0.000164180753586</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1.023</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="P13" t="n">
+        <v>1.756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>